<commit_message>
Exportación a excel con condicionales
</commit_message>
<xml_diff>
--- a/Scraping/google-play-scraper-FA (node)/scrapingReviewsFeelings.xlsx
+++ b/Scraping/google-play-scraper-FA (node)/scrapingReviewsFeelings.xlsx
@@ -32,12 +32,27 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00008000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -58,12 +73,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -450,19 +468,19 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>reviewCreatedVersion</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>content</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>thumbsUpCount</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>content</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>reviewCreatedVersion</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>score</t>
@@ -470,7 +488,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>puntuaciónSentimientos</t>
+          <t>feelingScore</t>
         </is>
       </c>
     </row>
@@ -483,23 +501,23 @@
       <c r="B2" s="2" t="n">
         <v>44594.64815972222</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>6.6.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cumple su función, eso sí cómo dato estaría muy bien que se te notificara cuándo las Actas se modifican. Por otro lado, también estaría bien que pudiera acceder al horario individual de cada alumno. Pd: Subid también la app a Appgallery</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>8</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>fulfills function, although data would good notified minutes modified . hand, would also nice could access individual schedule student . ps: also upload app appgallery</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>6.6.0</t>
-        </is>
       </c>
       <c r="F2" t="n">
         <v>5</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.4333333333333333, subjectivity=0.6666666666666666)</t>
         </is>
@@ -514,23 +532,23 @@
       <c r="B3" s="2" t="n">
         <v>43635.86333333333</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Me parece bastante útil, pero casi pongo las 5 estrellas porque, ya que puedes visualizar tu codigo de la tarjeta, se podria habilitar la proximidad del movil como si fuese la misma tarjeta con el campo magnetico (para las puertas de la ESI por ejemplo), y por otro lado puedes visualizar tu expediente con las notas solo, pero estaria bien que se pudiese ver mas cosas como matricula, datos bancarios, etc. Pero por todo lo demas, lo veo bastante completo ?</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>11</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>find quite useful, almost put 5 stars, since see card code, proximity mobile could enabled card magnetic field (doors esi example), hand view file notes alone, would nice could see things enrollment, bank details, etc . everything else, see quite complete?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F3" t="n">
         <v>4</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.3333333333333333, subjectivity=0.4666666666666666)</t>
         </is>
@@ -545,23 +563,23 @@
       <c r="B4" s="2" t="n">
         <v>43699.94783564815</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>La idea está bastante bien y resulta cómodo tener todo lo relativo a la UCA en una sola app, pero se queda muy pillada y cuando intento acceder ya sea al campus o a webmerlín se cierra sola, no sé si será culpa de mi móvil o si le pasa a más gente. Por otra parte, no me gusta que me pidan acceso a mis datos del banco, y en cuanto a los retos está bastante entretenido, pero deberían informar del ganador más rápido. Si arreglaran los fallitos para que no se cierre la app sola le daría 5 estrellas.</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>2</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>idea quite good's convenient everything related uca single app, gets stuck try access either campus webmerlin closes,n't know's mobile's fault happens people . hand,n't like asked access bank details, challenges,'s quite entertaining, report winner faster . fixed bugs appn't close, would give 5 stars.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F4" t="n">
         <v>4</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.24571428571428572, subjectivity=0.4228571428571429)</t>
         </is>
@@ -576,23 +594,23 @@
       <c r="B5" s="2" t="n">
         <v>43638.67614583333</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Muy buena, estaria genial que enviará notificaciones cuando se suban notas al acta, así como sugerencia. Y que se pudiera ver el horario de revisiones, que si se puede ver desde PC Por lo demas muy bien, ya era hora.</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>good, would great send notifications notes uploaded minutes, well suggestions . could see schedule reviews, see pc rest well,'s time.</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F5" t="n">
         <v>4</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.75, subjectivity=0.675)</t>
         </is>
@@ -607,23 +625,23 @@
       <c r="B6" s="2" t="n">
         <v>43624.8953125</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Buena, pero con fallos, a veces se queda pillada y le falta aun por mejorar,(ya que se puede ver el correo, debería haber una opción para la biblioteca) me parece una idea genial y cuando mejore se llevara las 5 estrellas ??</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>4</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>good, bugs, sometimes gets caught still needs improved, (since see mail, option library) think's great idea improves get 5 stars??</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F6" t="n">
         <v>3</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.75, subjectivity=0.675)</t>
         </is>
@@ -638,23 +656,23 @@
       <c r="B7" s="2" t="n">
         <v>43627.42532407407</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>¡Lo que necesitabamos! Esta genial, incluye tarjeta virtual, email Webmerlin, Campus virtual, Calificaciones, Directorio...ojalá notificaran cada vez que ponen alguna nota nueva, o llega algún correo, por lo demás, perfecta.</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>6</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>needed!'s great, includes virtual card, webmerlin email, virtual campus, qualifications, directory...wish would notify every time put new note, email arrives, otherwise, perfect.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F7" t="n">
         <v>5</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.6454545454545455, subjectivity=0.7348484848484849)</t>
         </is>
@@ -669,23 +687,23 @@
       <c r="B8" s="2" t="n">
         <v>43633.41778935185</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>useful app important thing missing, notifications . notified put note, would totally useful.</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Es una app muy útil pero falta lo más importante, LAS NOTIFICACIONES. Si notificase cuando ponen una nota ya sí que sería de una utilidad total.</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>4</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.19999999999999998, subjectivity=0.2625)</t>
         </is>
@@ -700,23 +718,23 @@
       <c r="B9" s="2" t="n">
         <v>43641.48234953704</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>good application although give 5 stars notify uploaded note section notes, rest great although sometimes hangs</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>es una aplicación muy buena aunque le daré 5 estrellas cuando avisen de que han subido una nota en el apartado de mis notas, por el resto genial aunque a veces se cuelga</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>4</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.75, subjectivity=0.675)</t>
         </is>
@@ -731,23 +749,23 @@
       <c r="B10" s="2" t="n">
         <v>44130.74974537037</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>6.5.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Todos los días se aprende cosas nuevas. Gracias al esfuerzo de todos avanzamos con buen rumbo. Esta aplicación me ayudo a acceder al portal de la UCA con más facilidad. Me gusta mucho.</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>3</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>every day learn new things . thanks everyone's efforts, moving right direction . application helped access uca portal easily . like lot.</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>6.5.0</t>
-        </is>
       </c>
       <c r="F10" t="n">
         <v>5</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.26385281385281384, subjectivity=0.5058982683982685)</t>
         </is>
@@ -762,23 +780,23 @@
       <c r="B11" s="2" t="n">
         <v>43633.37861111111</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Por ahora bien No me da fallo, desconozco si gastará mucha batería o no, pero me resulta interesante ver como ha podido agruparlo todo ne una sola aplicación. Por ahora muy bien UCA</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>2</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>far goodn't give failure,n't know use lot battery, find interesting see able group everything single application . far good uca</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F11" t="n">
         <v>5</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.27648809523809526, subjectivity=0.6049107142857144)</t>
         </is>
@@ -793,23 +811,23 @@
       <c r="B12" s="2" t="n">
         <v>43629.04681712963</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>No me deja entrar dice que mis datos son incorrectos cuando hasta hace un rato estaba utilizando la app sin ningún problema! arreglenlo porque en épocas d exámenes es muy importante está app</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
         <v>8</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>won't let enter says data incorrect ago using app without problem! fix times exams app important</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.4, subjectivity=1.0)</t>
         </is>
@@ -824,23 +842,23 @@
       <c r="B13" s="2" t="n">
         <v>43715.79381944444</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>6.0.11</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Genial aplicación de la UCA, puedes estar al día de todas las cosas con un simple click, ver tus notas, etc.</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
         <v>3</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>great application uca, keep date everything simple click, see notes, etc.</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>6.0.11</t>
-        </is>
       </c>
       <c r="F13" t="n">
         <v>5</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.4, subjectivity=0.5535714285714286)</t>
         </is>
@@ -855,23 +873,23 @@
       <c r="B14" s="2" t="n">
         <v>43630.96158564815</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>idea good, banco santander involved...use personal data, much . rest everything correct good idea.</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>La idea es buena, que este el Banco Santander metido... y que puedan llegar a utilizar tus datos personales, no tanto. Por lo demas todo correcto y una buena idea.</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.39999999999999997, subjectivity=0.42500000000000004)</t>
         </is>
@@ -886,23 +904,23 @@
       <c r="B15" s="2" t="n">
         <v>44102.54403935185</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>6.4.5</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Soy una estudiante de la UCA y esta aplicacion ayuda bastante y es facil de usar.ademas facilita el acceso de las notas y agenda.</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
         <v>1</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>student uca application helps lot easy use . also facilitates access notes agenda.</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>6.4.5</t>
-        </is>
       </c>
       <c r="F15" t="n">
         <v>5</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.43333333333333335, subjectivity=0.8333333333333334)</t>
         </is>
@@ -917,23 +935,23 @@
       <c r="B16" s="2" t="n">
         <v>43644.68815972222</v>
       </c>
-      <c r="C16" t="n">
-        <v>0</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>practice simplify pages uca student usually visits mobile.</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Práctica y simplifica todas las páginas que un alumno de la UCA suele visitar desde su móvil.</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>4</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.25, subjectivity=0.25)</t>
         </is>
@@ -948,23 +966,23 @@
       <c r="B17" s="2" t="n">
         <v>44434.95059027777</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>6.9.0</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Cuando me meto en "mis notas" me aparecen todas suspensas. Podrían arreglarlo cuanto antes, gracias ?</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>29</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>go "notes" appear suspended . could fix soon possible, thanks?</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>6.9.0</t>
-        </is>
       </c>
       <c r="F17" t="n">
         <v>3</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.1, subjectivity=0.6)</t>
         </is>
@@ -979,23 +997,23 @@
       <c r="B18" s="2" t="n">
         <v>44595.53128472222</v>
       </c>
-      <c r="C18" t="n">
-        <v>0</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>6.12.0</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>lot advertising little utility</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>6.12.0</t>
-        </is>
+          <t>Mucha publicidad y poca utilidad</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.1875, subjectivity=0.5)</t>
         </is>
@@ -1010,23 +1028,23 @@
       <c r="B19" s="2" t="n">
         <v>44588.1415625</v>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>6.11.1</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>garbage application, works shame . make app conditions uca already much bad fame . give 1 star can't leave blank.</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>6.11.1</t>
-        </is>
+          <t>Vaya basura de aplicación, funciona de pena. Hagan una app en condiciones que demasiada mala fama tiene ya la UCA. Y le doy 1 estrella porque no la puedo dejar en blanco.</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.3499999999999999, subjectivity=0.3333333333333333)</t>
         </is>
@@ -1041,23 +1059,23 @@
       <c r="B20" s="2" t="n">
         <v>44629.76700231482</v>
       </c>
-      <c r="C20" t="n">
-        <v>0</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>6.12.1</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>app height great university.</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>6.12.1</t>
-        </is>
+          <t>Una app a la altura de esta gran Universidad.</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>5</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.8, subjectivity=0.75)</t>
         </is>
@@ -1072,23 +1090,23 @@
       <c r="B21" s="2" t="n">
         <v>44540.95178240741</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>6.11.0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Ha dejado de funcionar la tarjeta virtual</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>1</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>virtual card stopped working</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>6.11.0</t>
-        </is>
       </c>
       <c r="F21" t="n">
         <v>3</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1103,23 +1121,23 @@
       <c r="B22" s="2" t="n">
         <v>44038.60899305555</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>6.4.1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Muy chula, y especialmente útil para mirar las calificaciones de las actas con un simple click</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>2</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>cool, especially useful see qualifications minutes simple click</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>6.4.1</t>
-        </is>
       </c>
       <c r="F22" t="n">
         <v>5</v>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.31666666666666665, subjectivity=0.3357142857142857)</t>
         </is>
@@ -1134,23 +1152,23 @@
       <c r="B23" s="2" t="n">
         <v>43899.43957175926</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>6.2.0</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Una aplicación muy intuitiva y bastante util hoy en dia!</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
         <v>2</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>intuitive quite useful application today!</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>6.2.0</t>
-        </is>
       </c>
       <c r="F23" t="n">
         <v>5</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.375, subjectivity=0.0)</t>
         </is>
@@ -1165,23 +1183,23 @@
       <c r="B24" s="2" t="n">
         <v>43720.54355324074</v>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>6.0.11</t>
+        </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>thingn't like go see grades, last year saw saved, first one enrolled.</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>6.0.11</t>
-        </is>
+          <t>Lo único que no me gusta es que cuando vas a ver las notas, no se guarda el último año que viste, sino el primero en el que te matriculaste.</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
       </c>
       <c r="F24" t="n">
         <v>4</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.125, subjectivity=0.19999999999999998)</t>
         </is>
@@ -1196,23 +1214,23 @@
       <c r="B25" s="2" t="n">
         <v>43717.9033449074</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>6.0.11</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>La actualización ha hecho que la App sea mucho peor qur anteriormente. Era de esperar viniendo de la UCA.</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
         <v>4</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>update made app much worse . expected coming uca.</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>6.0.11</t>
-        </is>
       </c>
       <c r="F25" t="n">
         <v>1</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.25, subjectivity=0.5)</t>
         </is>
@@ -1227,23 +1245,23 @@
       <c r="B26" s="2" t="n">
         <v>43625.82039351852</v>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>comfortable easy use . totally recommended.</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Cómoda y fácil de usar. Totalmente recomendable.</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
       </c>
       <c r="F26" t="n">
         <v>4</v>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.2777777777777778, subjectivity=0.7944444444444444)</t>
         </is>
@@ -1258,23 +1276,23 @@
       <c r="B27" s="2" t="n">
         <v>43623.52315972222</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>muy eficiente perfecta para estudiantes puedes disponer hasta de la tarjeta de la uca si la pierdes</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
         <v>1</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>efficient perfect students even uca card lose</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F27" t="n">
         <v>5</v>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=1.0, subjectivity=1.0)</t>
         </is>
@@ -1289,23 +1307,23 @@
       <c r="B28" s="2" t="n">
         <v>43712.83795138889</v>
       </c>
-      <c r="C28" t="n">
-        <v>0</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>6.0.11</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>lacks many improvements, still grow</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>6.0.11</t>
-        </is>
+          <t>Le faltan muchas mejoras, le queda aún por crecer</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
       </c>
       <c r="F28" t="n">
         <v>3</v>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.5, subjectivity=0.5)</t>
         </is>
@@ -1320,23 +1338,23 @@
       <c r="B29" s="2" t="n">
         <v>44181.87998842593</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>6.5.2</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Cumple con su función, no está mal. Estaría bien que pudiese tener el horario del curso también.</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
         <v>6</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>job, bad . would nice could course schedule well.</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>6.5.2</t>
-        </is>
       </c>
       <c r="F29" t="n">
         <v>5</v>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G29" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.04999999999999993, subjectivity=0.8333333333333333)</t>
         </is>
@@ -1351,23 +1369,23 @@
       <c r="B30" s="2" t="n">
         <v>43773.58197916667</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>6.0.14</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Increíble aplicación pero una oportunidad desaprovechada para hacer un maravilloso juego de palabras. 8/10</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
         <v>3</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>amazing app missed opportunity make wonderful pun . 8/10</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>6.0.14</t>
-        </is>
       </c>
       <c r="F30" t="n">
         <v>4</v>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.8, subjectivity=0.95)</t>
         </is>
@@ -1382,23 +1400,23 @@
       <c r="B31" s="2" t="n">
         <v>43731.91162037037</v>
       </c>
-      <c r="C31" t="n">
-        <v>0</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>6.0.12</t>
+        </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>lack access campus things improve, idea good development worthwhile.</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>6.0.12</t>
-        </is>
+          <t>Falta acceso al campus y otras cosas que mejorar, pero la idea es buena y su desarrollo merece la pena.</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
       </c>
       <c r="F31" t="n">
         <v>5</v>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G31" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.6, subjectivity=0.55)</t>
         </is>
@@ -1413,23 +1431,23 @@
       <c r="B32" s="2" t="n">
         <v>43638.37414351852</v>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>comfortable . would add option see schedules</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Muy cómoda. Añadiría la opción de ver horarios</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>4</v>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G32" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.4, subjectivity=0.8)</t>
         </is>
@@ -1444,23 +1462,23 @@
       <c r="B33" s="2" t="n">
         <v>43733.57310185185</v>
       </c>
-      <c r="C33" t="n">
-        <v>0</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>6.0.12</t>
+        </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>could put last year studied review grades subjects, first year</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>6.0.12</t>
-        </is>
+          <t>Te podría poner el último año cursado cuando revisas las notas de las asignaturas, no el primer curso</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
       </c>
       <c r="F33" t="n">
         <v>3</v>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.125, subjectivity=0.19999999999999998)</t>
         </is>
@@ -1475,23 +1493,23 @@
       <c r="B34" s="2" t="n">
         <v>43627.09704861111</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Le faltan lootboxes</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
         <v>2</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>missing lootboxes</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F34" t="n">
         <v>4</v>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.2, subjectivity=0.05)</t>
         </is>
@@ -1506,23 +1524,23 @@
       <c r="B35" s="2" t="n">
         <v>43626.5116550926</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>No puedo acceder con usuario y contraseña...</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
         <v>3</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>can't access username password ...</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
       </c>
       <c r="F35" t="n">
         <v>1</v>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1537,23 +1555,23 @@
       <c r="B36" s="2" t="n">
         <v>43633.86540509259</v>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>lacks link access file download certificate</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>solo le falta un enlace para acceder al expediente y descargar el certificado</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>4</v>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1568,23 +1586,23 @@
       <c r="B37" s="2" t="n">
         <v>44437.50233796296</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>6.9.0</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Desde hace unos meses la app no me funciona</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
         <v>2</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>months app work</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>6.9.0</t>
-        </is>
       </c>
       <c r="F37" t="n">
         <v>1</v>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="G37" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1599,23 +1617,23 @@
       <c r="B38" s="2" t="n">
         <v>43660.78943287037</v>
       </c>
-      <c r="C38" t="n">
-        <v>0</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>simple, although usually falls</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Sencilla,aunque se suele caer</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
       </c>
       <c r="F38" t="n">
         <v>4</v>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="G38" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.125, subjectivity=0.3035714285714286)</t>
         </is>
@@ -1630,23 +1648,23 @@
       <c r="B39" s="2" t="n">
         <v>43717.84048611111</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>6.0.11</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>No me deja entrar en la app con mi usuario y contraseña.</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
         <v>3</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>won't let enter app username password.</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>6.0.11</t>
-        </is>
       </c>
       <c r="F39" t="n">
         <v>1</v>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="G39" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1661,23 +1679,23 @@
       <c r="B40" s="2" t="n">
         <v>43630.53115740741</v>
       </c>
-      <c r="C40" t="n">
-        <v>0</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>would nice access virtual campus therefore subjects</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>estaría bien que tuviera acceso al campus virtual y por ello a las asignaturas</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
       </c>
       <c r="F40" t="n">
         <v>3</v>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G40" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.6, subjectivity=1.0)</t>
         </is>
@@ -1692,23 +1710,23 @@
       <c r="B41" s="2" t="n">
         <v>44232.88297453704</v>
       </c>
-      <c r="C41" t="n">
-        <v>0</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>6.6.0</t>
+        </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>good, necessary information.</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>6.6.0</t>
-        </is>
+          <t>Muy buen, toda la información necesaria.</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
       </c>
       <c r="F41" t="n">
         <v>5</v>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="G41" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.35, subjectivity=0.8)</t>
         </is>
@@ -1723,23 +1741,23 @@
       <c r="B42" s="2" t="n">
         <v>43717.52980324074</v>
       </c>
-      <c r="C42" t="n">
-        <v>0</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>6.0.11</t>
+        </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>observations missing ratings</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>6.0.11</t>
-        </is>
+          <t>Faltan las observaciones en las calificaciones</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
       </c>
       <c r="F42" t="n">
         <v>3</v>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G42" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.2, subjectivity=0.05)</t>
         </is>
@@ -1754,23 +1772,23 @@
       <c r="B43" s="2" t="n">
         <v>44452.595625</v>
       </c>
-      <c r="C43" t="n">
-        <v>0</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>6.9.0</t>
+        </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>sometimes saturates responds</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>6.9.0</t>
-        </is>
+          <t>Veces si satura pero después responde</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
       </c>
       <c r="F43" t="n">
         <v>5</v>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="G43" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1785,23 +1803,23 @@
       <c r="B44" s="2" t="n">
         <v>43629.56109953704</v>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>useful . nice job</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Muy útil. Buen trabajo</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>5</v>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="G44" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.44999999999999996, subjectivity=0.5)</t>
         </is>
@@ -1816,23 +1834,23 @@
       <c r="B45" s="2" t="n">
         <v>43735.02987268518</v>
       </c>
-      <c r="C45" t="n">
-        <v>0</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>6.0.12</t>
+        </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>virtual campus closed</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>6.0.12</t>
-        </is>
+          <t>Se cierra el campus virtual</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>2</v>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="G45" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=-0.1, subjectivity=0.1)</t>
         </is>
@@ -1847,23 +1865,23 @@
       <c r="B46" s="2" t="n">
         <v>43789.93585648148</v>
       </c>
-      <c r="C46" t="n">
-        <v>0</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>6.1.0</t>
+        </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>come suspended subjects? please fix</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>6.1.0</t>
-        </is>
+          <t>Por que sale que estoy suspenso en todas las asignaturas?? Arreglenlo porfa</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
       </c>
       <c r="F46" t="n">
         <v>2</v>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G46" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1878,23 +1896,23 @@
       <c r="B47" s="2" t="n">
         <v>44426.49619212963</v>
       </c>
-      <c r="C47" t="n">
-        <v>0</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>6.9.0</t>
+        </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>lot stress bro</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>6.9.0</t>
-        </is>
+          <t>Mucho estrés Bro</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
       </c>
       <c r="F47" t="n">
         <v>1</v>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="G47" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1909,23 +1927,23 @@
       <c r="B48" s="2" t="n">
         <v>44487.56636574074</v>
       </c>
-      <c r="C48" t="n">
-        <v>0</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>6.10.0</t>
+        </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>good</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>6.10.0</t>
-        </is>
+          <t>Muy bie</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
       </c>
       <c r="F48" t="n">
         <v>5</v>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="G48" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.7, subjectivity=0.6000000000000001)</t>
         </is>
@@ -1940,23 +1958,23 @@
       <c r="B49" s="2" t="n">
         <v>44467.88884259259</v>
       </c>
-      <c r="C49" t="n">
-        <v>0</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>6.8.2</t>
+        </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>yeeee</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>6.8.2</t>
-        </is>
+          <t>Yeeee</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
       </c>
       <c r="F49" t="n">
         <v>5</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -1971,23 +1989,23 @@
       <c r="B50" s="2" t="n">
         <v>44318.1006712963</v>
       </c>
-      <c r="C50" t="n">
-        <v>0</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>6.7.1</t>
+        </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>genial</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>6.7.1</t>
-        </is>
+          <t>Genial</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
       </c>
       <c r="F50" t="n">
         <v>5</v>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G50" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -2002,23 +2020,23 @@
       <c r="B51" s="2" t="n">
         <v>44137.88305555555</v>
       </c>
-      <c r="C51" t="n">
-        <v>0</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>6.5.0</t>
+        </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>good</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>6.5.0</t>
-        </is>
+          <t>Buena</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
       </c>
       <c r="F51" t="n">
         <v>5</v>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="G51" s="5" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.7, subjectivity=0.6000000000000001)</t>
         </is>
@@ -2033,23 +2051,23 @@
       <c r="B52" s="2" t="n">
         <v>44099.04413194444</v>
       </c>
-      <c r="C52" t="n">
-        <v>0</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>6.4.1</t>
+        </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>genial</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>6.4.1</t>
-        </is>
+          <t>Genial</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
       </c>
       <c r="F52" t="n">
         <v>5</v>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>
@@ -2064,23 +2082,23 @@
       <c r="B53" s="2" t="n">
         <v>43652.77194444444</v>
       </c>
-      <c r="C53" t="n">
-        <v>0</v>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>many upsets?</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>muchos disgustos ?</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
       </c>
       <c r="F53" t="n">
         <v>3</v>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.5, subjectivity=0.5)</t>
         </is>
@@ -2095,23 +2113,23 @@
       <c r="B54" s="2" t="n">
         <v>43626.77854166667</v>
       </c>
-      <c r="C54" t="n">
-        <v>0</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>love</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>Me encanta</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
       </c>
       <c r="F54" t="n">
         <v>5</v>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="G54" s="3" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.5, subjectivity=0.6)</t>
         </is>
@@ -2126,23 +2144,23 @@
       <c r="B55" s="2" t="n">
         <v>43638.35978009259</v>
       </c>
-      <c r="C55" t="n">
-        <v>0</v>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>5.7.9</t>
+        </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>well</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>5.7.9</t>
-        </is>
+          <t>muy bien</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
       </c>
       <c r="F55" t="n">
         <v>4</v>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G55" s="4" t="inlineStr">
         <is>
           <t>Sentiment(polarity=0.0, subjectivity=0.0)</t>
         </is>

</xml_diff>